<commit_message>
fix insert words in db using excel sheet
</commit_message>
<xml_diff>
--- a/populate/words.xlsx
+++ b/populate/words.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nodejs\who-is-undercover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\common\Desktop\Code\undercover\populate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49A2536-EC46-4F65-9552-989302ED7D30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{60E5C61E-3573-4D78-BCF9-06B87FF2C01F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="chinese" sheetId="2" r:id="rId1"/>
     <sheet name="english" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="234">
   <si>
     <t>初恋</t>
   </si>
@@ -725,12 +724,15 @@
   </si>
   <si>
     <t>glass</t>
+  </si>
+  <si>
+    <t>inserted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1128,19 +1130,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0585F02-79B5-466B-B275-8B18A2A6C1C4}">
-  <dimension ref="A1:C98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -1151,7 +1153,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -1162,7 +1164,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -1173,7 +1175,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -1184,7 +1186,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1195,7 +1197,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1206,7 +1208,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -1228,7 +1230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -1239,7 +1241,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -1250,7 +1252,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -1261,7 +1263,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -1272,7 +1274,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -1283,7 +1285,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -1294,7 +1296,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -1305,7 +1307,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -1316,7 +1318,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -1327,7 +1329,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -1338,7 +1340,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -1349,7 +1351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1360,7 +1362,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1371,7 +1373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1382,7 +1384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -1393,7 +1395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -1404,7 +1406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -1415,7 +1417,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -1426,7 +1428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -1437,7 +1439,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -1448,7 +1450,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -1459,7 +1461,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -1470,7 +1472,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -1481,7 +1483,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -1492,7 +1494,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -1503,7 +1505,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -1514,7 +1516,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -1525,7 +1527,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -1536,7 +1538,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -1547,7 +1549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -1558,7 +1560,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -1569,7 +1571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -1580,7 +1582,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -1591,7 +1593,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -1602,7 +1604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -1613,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -1624,7 +1626,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45</v>
       </c>
@@ -1635,7 +1637,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -1646,7 +1648,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>48</v>
       </c>
@@ -1668,7 +1670,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>49</v>
       </c>
@@ -1679,7 +1681,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>50</v>
       </c>
@@ -1690,7 +1692,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>51</v>
       </c>
@@ -1701,7 +1703,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>52</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>53</v>
       </c>
@@ -1723,7 +1725,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>54</v>
       </c>
@@ -1734,7 +1736,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>55</v>
       </c>
@@ -1745,7 +1747,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>56</v>
       </c>
@@ -1756,7 +1758,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>57</v>
       </c>
@@ -1767,7 +1769,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>58</v>
       </c>
@@ -1778,7 +1780,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>59</v>
       </c>
@@ -1789,7 +1791,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>60</v>
       </c>
@@ -1800,7 +1802,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>61</v>
       </c>
@@ -1811,7 +1813,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>62</v>
       </c>
@@ -1822,7 +1824,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>63</v>
       </c>
@@ -1833,7 +1835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>64</v>
       </c>
@@ -1844,7 +1846,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>65</v>
       </c>
@@ -1855,7 +1857,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>66</v>
       </c>
@@ -1866,7 +1868,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>67</v>
       </c>
@@ -1877,7 +1879,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>68</v>
       </c>
@@ -1888,7 +1890,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>69</v>
       </c>
@@ -1899,7 +1901,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>70</v>
       </c>
@@ -1910,7 +1912,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>71</v>
       </c>
@@ -1921,7 +1923,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>72</v>
       </c>
@@ -1932,7 +1934,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>73</v>
       </c>
@@ -1943,7 +1945,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>74</v>
       </c>
@@ -1954,7 +1956,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>75</v>
       </c>
@@ -1965,7 +1967,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>76</v>
       </c>
@@ -1976,7 +1978,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>77</v>
       </c>
@@ -1987,7 +1989,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>78</v>
       </c>
@@ -1998,7 +2000,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>79</v>
       </c>
@@ -2009,7 +2011,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>80</v>
       </c>
@@ -2020,7 +2022,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>81</v>
       </c>
@@ -2031,7 +2033,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>82</v>
       </c>
@@ -2042,7 +2044,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>83</v>
       </c>
@@ -2053,7 +2055,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>84</v>
       </c>
@@ -2064,7 +2066,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>85</v>
       </c>
@@ -2075,7 +2077,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>86</v>
       </c>
@@ -2086,7 +2088,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>87</v>
       </c>
@@ -2097,7 +2099,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>88</v>
       </c>
@@ -2108,7 +2110,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>89</v>
       </c>
@@ -2119,7 +2121,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>90</v>
       </c>
@@ -2130,7 +2132,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>91</v>
       </c>
@@ -2141,7 +2143,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>92</v>
       </c>
@@ -2152,7 +2154,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>93</v>
       </c>
@@ -2163,7 +2165,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>94</v>
       </c>
@@ -2174,7 +2176,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>95</v>
       </c>
@@ -2185,7 +2187,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>96</v>
       </c>
@@ -2196,7 +2198,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>97</v>
       </c>
@@ -2207,7 +2209,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>98</v>
       </c>
@@ -2216,6 +2218,9 @@
       </c>
       <c r="C98" s="1" t="s">
         <v>210</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2228,20 +2233,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D2669E-5129-48E0-B150-9D1272E8D56D}">
-  <dimension ref="A1:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1001</v>
       </c>
@@ -2252,7 +2257,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1002</v>
       </c>
@@ -2263,7 +2268,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1003</v>
       </c>
@@ -2274,7 +2279,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1004</v>
       </c>
@@ -2285,7 +2290,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1005</v>
       </c>
@@ -2296,7 +2301,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1006</v>
       </c>
@@ -2307,7 +2312,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1007</v>
       </c>
@@ -2318,7 +2323,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1008</v>
       </c>
@@ -2329,7 +2334,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1009</v>
       </c>
@@ -2340,7 +2345,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1010</v>
       </c>
@@ -2351,7 +2356,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1011</v>
       </c>
@@ -2362,7 +2367,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1012</v>
       </c>
@@ -2373,7 +2378,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1013</v>
       </c>
@@ -2384,7 +2389,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1014</v>
       </c>
@@ -2395,7 +2400,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1015</v>
       </c>
@@ -2406,7 +2411,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1016</v>
       </c>
@@ -2417,7 +2422,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1017</v>
       </c>
@@ -2428,7 +2433,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1018</v>
       </c>
@@ -2439,7 +2444,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1019</v>
       </c>
@@ -2450,7 +2455,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1020</v>
       </c>
@@ -2461,7 +2466,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1021</v>
       </c>
@@ -2472,7 +2477,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1022</v>
       </c>
@@ -2483,7 +2488,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1023</v>
       </c>
@@ -2492,6 +2497,9 @@
       </c>
       <c r="C23" s="1" t="s">
         <v>232</v>
+      </c>
+      <c r="D23" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>